<commit_message>
added sp names to read and write excel
</commit_message>
<xml_diff>
--- a/Adriatic/Adriatic_v3.xlsx
+++ b/Adriatic/Adriatic_v3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="6" activeTab="16"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -8524,7 +8524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
@@ -36987,10 +36987,15 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -37053,13 +37058,13 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -37085,13 +37090,13 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -37117,13 +37122,13 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -37152,13 +37157,13 @@
         <v>2</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -37187,13 +37192,13 @@
         <v>3</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -44229,7 +44234,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>